<commit_message>
TP de Diseño de Sistemas
</commit_message>
<xml_diff>
--- a/Excel/Alex The Analyst Course-Excel/XLOOKUP Excel Tutorial File.xlsx
+++ b/Excel/Alex The Analyst Course-Excel/XLOOKUP Excel Tutorial File.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fede Cocimano\Documents\ROAD-TO-DATA-CAREER\StarkIndustries-SpecialProjects\Excel\Alex The Analyst Course\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fede Cocimano\Documents\The Power Of The Sun In The Palm Of My Hand\StarkIndustries-Projects\-ProjectsAndPractice-\Excel\Alex The Analyst Course-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5020D7-FE00-48F4-8019-0DBFCA3E4861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7998265-0EE7-40EC-A3F3-EBD628398A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -398,13 +398,13 @@
       <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -498,9 +498,9 @@
     <tableColumn id="6" xr3:uid="{40081C4B-03B1-4D5B-A0CC-D74E361780CB}" name="Gender"/>
     <tableColumn id="7" xr3:uid="{9A1B323B-A13D-446C-8293-68D9DB1C32B5}" name="JobTitle"/>
     <tableColumn id="8" xr3:uid="{00C26AB8-C4FC-47F5-AC75-1D5578D131E2}" name="Salary"/>
-    <tableColumn id="9" xr3:uid="{8CBE6995-8C3A-48C8-9D13-14DBDD8ACF10}" name="StartDate" dataDxfId="8" totalsRowDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{0A9AEA38-C2C7-466D-A5F1-1FB69E7EB3CE}" name="EndDate" dataDxfId="7" totalsRowDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{ED00F26A-B9A5-4567-89C9-00C1A956B13C}" name="Email" dataDxfId="6" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{8CBE6995-8C3A-48C8-9D13-14DBDD8ACF10}" name="StartDate" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{0A9AEA38-C2C7-466D-A5F1-1FB69E7EB3CE}" name="EndDate" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{ED00F26A-B9A5-4567-89C9-00C1A956B13C}" name="Email" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -572,9 +572,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -612,7 +612,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -718,7 +718,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -860,7 +860,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3033,7 +3033,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>